<commit_message>
Added some notes in Documentation
Added some notes in Documentation
</commit_message>
<xml_diff>
--- a/documentation/Progress Sheet.xlsx
+++ b/documentation/Progress Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Mella\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C15A6D3-76A3-4809-9599-8EA7C5DA2ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FD278C-5FF4-4CDC-AEA4-3237FF31376B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A495D97C-BDD4-45C3-9E48-A1530F9CB0D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Code Path</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>No Light, It just blink</t>
+  </si>
+  <si>
+    <t>Compiled (Not able to verify as WiFi is not connected yet</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="B4:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,12 +552,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>